<commit_message>
删除 app/controller/word.php 中无用代码,增加注释 phpspreadsheet从1.25降到1.19 phpword从1.1升到1.3 增加tcpdf,mpdf等pdf库 风险研判模板更新 更新reportwork引用文件
</commit_message>
<xml_diff>
--- a/public/公司风险研判签到表模板.xlsx
+++ b/public/公司风险研判签到表模板.xlsx
@@ -29,7 +29,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
-    <t>乙烯分公司                        会议时间： 2023 年    月    日</t>
+    <t>乙烯分公司                        会议时间：      年    月    日</t>
   </si>
   <si>
     <t>参会单位</t>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>

</xml_diff>